<commit_message>
latest data. updated qc script to not have to rerun permutations for old participants. created the main analysis script
</commit_message>
<xml_diff>
--- a/results/qc_check_sheets/qc_check_debrief_and_errors.xlsx
+++ b/results/qc_check_sheets/qc_check_debrief_and_errors.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\levan\GitHub\fast_schema_analysis_3\results\qc_check_sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C064B003-2213-4DD9-B08A-A78593FA1480}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74E526E7-2216-40C3-9C56-71CA99D5CE92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
   <si>
     <t>participant</t>
   </si>
@@ -33,25 +33,22 @@
     <t>reason</t>
   </si>
   <si>
-    <t>sub_001</t>
-  </si>
-  <si>
-    <t>sub_002</t>
-  </si>
-  <si>
     <t>qc_fail_manual</t>
   </si>
   <si>
-    <t>sub_003</t>
-  </si>
-  <si>
-    <t>sub_004</t>
-  </si>
-  <si>
-    <t>sub_005</t>
-  </si>
-  <si>
-    <t>sub_006</t>
+    <t>sub_012</t>
+  </si>
+  <si>
+    <t>technical</t>
+  </si>
+  <si>
+    <t>sub_014</t>
+  </si>
+  <si>
+    <t>sub_020</t>
+  </si>
+  <si>
+    <t>missing input for listing names of pictures for the last page.</t>
   </si>
 </sst>
 </file>
@@ -375,75 +372,60 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:C86"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B2" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B3" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B4" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
         <v>7</v>
-      </c>
-      <c r="B6" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" t="b">
-        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>